<commit_message>
UPDATE: creacion de variables para outups, instalacion de plugin y macheo de las nuevas variables con el excel
</commit_message>
<xml_diff>
--- a/Resources/db_farmanet_escenarios.xlsx
+++ b/Resources/db_farmanet_escenarios.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alflopez-ext\Documents\Automation\Proyectos_Katalon\git\katalonProjects\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED8308F-8D28-4141-A560-A9F205D8E90D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65711AC2-FFBF-4490-8244-474E8337FEFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{DCE7E561-B195-4D45-B807-475C6552309D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DCE7E561-B195-4D45-B807-475C6552309D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="generador_datos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,22 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
-  <si>
-    <t>ambiente</t>
-  </si>
-  <si>
-    <t>materiales</t>
-  </si>
-  <si>
-    <t>comitente</t>
-  </si>
-  <si>
-    <t>trazable</t>
-  </si>
-  <si>
-    <t>tipo_material</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>filtrar</t>
   </si>
@@ -54,103 +39,130 @@
     <t>generar</t>
   </si>
   <si>
-    <t>mostrar</t>
-  </si>
-  <si>
-    <t>cant_ingresar</t>
-  </si>
-  <si>
-    <t>ingresa_cuarentena</t>
-  </si>
-  <si>
-    <t>codificacion</t>
-  </si>
-  <si>
-    <t>informado_por</t>
-  </si>
-  <si>
-    <t>ingresa_trazado</t>
-  </si>
-  <si>
-    <t>nac_trazado</t>
-  </si>
-  <si>
-    <t>procedencia</t>
-  </si>
-  <si>
-    <t>cod_aduana</t>
-  </si>
-  <si>
-    <t>cod_destino</t>
-  </si>
-  <si>
-    <t>n_despacho</t>
-  </si>
-  <si>
-    <t>dig_ver_n_despacho</t>
-  </si>
-  <si>
-    <t>fecha_despacho_plaza</t>
-  </si>
-  <si>
-    <t>prioridad</t>
-  </si>
-  <si>
-    <t>cod_plazo</t>
-  </si>
-  <si>
-    <t>canti_pedido</t>
-  </si>
-  <si>
-    <t>descuento</t>
-  </si>
-  <si>
-    <t>uni_bonificadas</t>
-  </si>
-  <si>
-    <t>otros_clientes</t>
-  </si>
-  <si>
-    <t>cliente_dist</t>
-  </si>
-  <si>
-    <t>ped_comitente_i101</t>
-  </si>
-  <si>
-    <t>ped_dist_i106</t>
-  </si>
-  <si>
-    <t>pedi_cliente_i089</t>
-  </si>
-  <si>
-    <t>rem_elect_i141</t>
-  </si>
-  <si>
-    <t>alta_lotes_i105</t>
-  </si>
-  <si>
-    <t>todas_formas_pago</t>
-  </si>
-  <si>
-    <t>mostrar_lotes</t>
-  </si>
-  <si>
-    <t>Novartis 06</t>
-  </si>
-  <si>
-    <t>crear_pedido</t>
-  </si>
-  <si>
     <t>ON</t>
   </si>
   <si>
     <t>OFF</t>
   </si>
   <si>
-    <t>ZPRO</t>
-  </si>
-  <si>
-    <t>SI</t>
+    <t>param_ambiente</t>
+  </si>
+  <si>
+    <t>param_materiales</t>
+  </si>
+  <si>
+    <t>param_comitente</t>
+  </si>
+  <si>
+    <t>param_trazable</t>
+  </si>
+  <si>
+    <t>param_crear_pedido</t>
+  </si>
+  <si>
+    <t>param_tipo_material</t>
+  </si>
+  <si>
+    <t>out_lote</t>
+  </si>
+  <si>
+    <t>out_fech_actual</t>
+  </si>
+  <si>
+    <t>out_fech_ven</t>
+  </si>
+  <si>
+    <t>out_n_remito</t>
+  </si>
+  <si>
+    <t>param_cant_ingresar</t>
+  </si>
+  <si>
+    <t>out_oc_comitente</t>
+  </si>
+  <si>
+    <t>param_ingresa_cuarentena</t>
+  </si>
+  <si>
+    <t>param_codificacion</t>
+  </si>
+  <si>
+    <t>param_informado_por</t>
+  </si>
+  <si>
+    <t>param_ingresa_trazado</t>
+  </si>
+  <si>
+    <t>param_nac_trazado</t>
+  </si>
+  <si>
+    <t>param_procedencia</t>
+  </si>
+  <si>
+    <t>param_cod_aduana</t>
+  </si>
+  <si>
+    <t>param_cod_destino</t>
+  </si>
+  <si>
+    <t>out_n_despacho</t>
+  </si>
+  <si>
+    <t>out_dig_ver_n_despacho</t>
+  </si>
+  <si>
+    <t>out_fecha_despacho_plaza</t>
+  </si>
+  <si>
+    <t>out_n_pedido</t>
+  </si>
+  <si>
+    <t>param_prioridad</t>
+  </si>
+  <si>
+    <t>param_cod_plazo</t>
+  </si>
+  <si>
+    <t>param_todas_formas_pago</t>
+  </si>
+  <si>
+    <t>param_canti_pedido</t>
+  </si>
+  <si>
+    <t>param_descuento</t>
+  </si>
+  <si>
+    <t>param_uni_bonificadas</t>
+  </si>
+  <si>
+    <t>param_otros_clientes</t>
+  </si>
+  <si>
+    <t>param_cliente_dist</t>
+  </si>
+  <si>
+    <t>out_alta_lotes_i105</t>
+  </si>
+  <si>
+    <t>out_rem_elect_i141</t>
+  </si>
+  <si>
+    <t>out_pedi_cliente_i089</t>
+  </si>
+  <si>
+    <t>out_ped_dist_i106</t>
+  </si>
+  <si>
+    <t>out_ped_comitente_i101</t>
+  </si>
+  <si>
+    <t>out_n_entrega</t>
+  </si>
+  <si>
+    <t>out_n_factura</t>
+  </si>
+  <si>
+    <t>out_n_orden_compra</t>
   </si>
   <si>
     <t>Calidad</t>
@@ -169,12 +181,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -189,8 +213,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,181 +531,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2E8823-6EAB-486E-9169-DE992862E70B}">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AQ2" sqref="AQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="22" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="22" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>1002</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="O2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="AD2">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W1" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2">
-        <v>2001</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2">
-        <v>19</v>
+      <c r="AG2">
+        <v>2032500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: agregado casos sap.
</commit_message>
<xml_diff>
--- a/Resources/db_farmanet_escenarios.xlsx
+++ b/Resources/db_farmanet_escenarios.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alflopez-ext\Documents\Automation\Proyectos_Katalon\git\katalonProjects\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65711AC2-FFBF-4490-8244-474E8337FEFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C4456E-BF93-40C5-A87D-240C0C4E676D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DCE7E561-B195-4D45-B807-475C6552309D}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>filtrar</t>
   </si>
@@ -166,13 +166,44 @@
   </si>
   <si>
     <t>Calidad</t>
+  </si>
+  <si>
+    <t>out_n_pedido_sap</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>LOTE1063</t>
+  </si>
+  <si>
+    <t>20200103</t>
+  </si>
+  <si>
+    <t>20210825</t>
+  </si>
+  <si>
+    <t>1063</t>
+  </si>
+  <si>
+    <t>0000-00001063</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>20191104</t>
+  </si>
+  <si>
+    <t>3406454</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,57 +562,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2E8823-6EAB-486E-9169-DE992862E70B}">
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AQ2" sqref="AQ2"/>
+      <selection activeCell="AI5" sqref="AI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="22" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="28.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="14.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="11" max="12" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="19" max="21" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="35" max="36" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -700,16 +730,19 @@
         <v>40</v>
       </c>
       <c r="AN1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -719,18 +752,50 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" t="s">
+        <v>50</v>
+      </c>
       <c r="M2">
         <v>10</v>
       </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
       <c r="O2" t="s">
         <v>3</v>
       </c>
+      <c r="W2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>54</v>
+      </c>
       <c r="AD2">
         <v>10</v>
       </c>
       <c r="AG2">
         <v>2032500</v>
       </c>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UPDATE: creacion casos, objetos, test suites y automatizacion trx
</commit_message>
<xml_diff>
--- a/Resources/db_farmanet_escenarios.xlsx
+++ b/Resources/db_farmanet_escenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alflopez-ext\Documents\Automation\Proyectos_Katalon\git\katalonProjects\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C4456E-BF93-40C5-A87D-240C0C4E676D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72045F5-098F-48C0-B2EB-C5F53A839B7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DCE7E561-B195-4D45-B807-475C6552309D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>filtrar</t>
   </si>
@@ -174,28 +174,40 @@
     <t/>
   </si>
   <si>
-    <t>LOTE1063</t>
-  </si>
-  <si>
-    <t>20200103</t>
-  </si>
-  <si>
-    <t>20210825</t>
-  </si>
-  <si>
-    <t>1063</t>
-  </si>
-  <si>
-    <t>0000-00001063</t>
+    <t>LOTE1093</t>
+  </si>
+  <si>
+    <t>20200107</t>
+  </si>
+  <si>
+    <t>20210829</t>
+  </si>
+  <si>
+    <t>1093</t>
+  </si>
+  <si>
+    <t>0000-00001093</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>20191104</t>
-  </si>
-  <si>
-    <t>3406454</t>
+    <t>20191108</t>
+  </si>
+  <si>
+    <t>3406757</t>
+  </si>
+  <si>
+    <t>LOTE1095</t>
+  </si>
+  <si>
+    <t>1095</t>
+  </si>
+  <si>
+    <t>0000-00001095</t>
+  </si>
+  <si>
+    <t>3406778</t>
   </si>
 </sst>
 </file>
@@ -562,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2E8823-6EAB-486E-9169-DE992862E70B}">
-  <dimension ref="A1:AQ2"/>
+  <dimension ref="A1:AQ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AI5" sqref="AI5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +590,7 @@
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
     <col min="11" max="12" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
@@ -753,7 +765,7 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="J2" t="s">
         <v>48</v>
@@ -762,13 +774,13 @@
         <v>49</v>
       </c>
       <c r="L2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="M2">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="O2" t="s">
         <v>3</v>
@@ -783,10 +795,10 @@
         <v>53</v>
       </c>
       <c r="Z2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AD2">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="AG2">
         <v>2032500</v>
@@ -797,6 +809,29 @@
       <c r="AL2"/>
       <c r="AM2"/>
     </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>1002</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>19</v>
+      </c>
+      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD3">
+        <v>19</v>
+      </c>
+      <c r="AG3">
+        <v>2032500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
UPDATE: creacion nuevos casos y test suites
</commit_message>
<xml_diff>
--- a/Resources/db_farmanet_escenarios.xlsx
+++ b/Resources/db_farmanet_escenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alflopez-ext\Documents\Automation\Proyectos_Katalon\git\katalonProjects\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72045F5-098F-48C0-B2EB-C5F53A839B7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF28D52-F0FA-44C8-912F-42C46F61EAF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DCE7E561-B195-4D45-B807-475C6552309D}"/>
+    <workbookView xWindow="735" yWindow="645" windowWidth="17475" windowHeight="9465" xr2:uid="{DCE7E561-B195-4D45-B807-475C6552309D}"/>
   </bookViews>
   <sheets>
     <sheet name="generador_datos" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>filtrar</t>
   </si>
@@ -171,43 +171,55 @@
     <t>out_n_pedido_sap</t>
   </si>
   <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>out_ref_externa</t>
+  </si>
+  <si>
+    <t>LOTE1125</t>
+  </si>
+  <si>
+    <t>20200115</t>
+  </si>
+  <si>
+    <t>20210906</t>
+  </si>
+  <si>
+    <t>1125</t>
+  </si>
+  <si>
+    <t>R0000-00001125</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>20191116</t>
+  </si>
+  <si>
+    <t>3407077</t>
+  </si>
+  <si>
+    <t>1002;LOTE1125;20210906;DESC LOTE1125;LOTE1125;N;LOTE1125;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001125;FNET;FNET;02;ZRET;20200115;;1800000122;20200115;08:00;16:00;20000;Remito electrónico Test;;;1002;27;C/U;LOTE1125;;;;;0000-00001125;1125;20200115;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200115002C001CLIENTESAPNROOC032202001151002              27           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202001150002073900PEDIDO                                                                          1002              27       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200115NROOC1  27     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              27     816 0  </t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>LOTE1093</t>
-  </si>
-  <si>
-    <t>20200107</t>
-  </si>
-  <si>
-    <t>20210829</t>
-  </si>
-  <si>
-    <t>1093</t>
-  </si>
-  <si>
-    <t>0000-00001093</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>20191108</t>
-  </si>
-  <si>
-    <t>3406757</t>
-  </si>
-  <si>
-    <t>LOTE1095</t>
-  </si>
-  <si>
-    <t>1095</t>
-  </si>
-  <si>
-    <t>0000-00001095</t>
-  </si>
-  <si>
-    <t>3406778</t>
+    <t>0001128513</t>
   </si>
 </sst>
 </file>
@@ -256,10 +268,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2E8823-6EAB-486E-9169-DE992862E70B}">
-  <dimension ref="A1:AQ3"/>
+  <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AN9" sqref="AN9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,13 +630,14 @@
     <col min="37" max="37" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
     <col min="38" max="38" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
     <col min="39" max="39" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="40" max="40" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -742,19 +756,22 @@
         <v>40</v>
       </c>
       <c r="AN1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -764,72 +781,68 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="M2">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="N2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="O2" t="s">
         <v>3</v>
       </c>
       <c r="W2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="X2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Y2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Z2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AD2">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="AG2">
         <v>2032500</v>
       </c>
-      <c r="AI2"/>
-      <c r="AJ2"/>
-      <c r="AK2"/>
-      <c r="AL2"/>
-      <c r="AM2"/>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3">
-        <v>1002</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <v>19</v>
-      </c>
-      <c r="O3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD3">
-        <v>19</v>
-      </c>
-      <c r="AG3">
-        <v>2032500</v>
+      <c r="AI2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN2">
+        <v>3407087</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPDATE: se16n, punto de arranque, iteraciones x cant de filas
</commit_message>
<xml_diff>
--- a/Resources/db_farmanet_escenarios.xlsx
+++ b/Resources/db_farmanet_escenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alflopez-ext\Documents\Automation\Proyectos_Katalon\git\katalonProjects\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF28D52-F0FA-44C8-912F-42C46F61EAF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D302DABB-D6C0-48D2-811C-A34EA549F945}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="645" windowWidth="17475" windowHeight="9465" xr2:uid="{DCE7E561-B195-4D45-B807-475C6552309D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{DCE7E561-B195-4D45-B807-475C6552309D}"/>
   </bookViews>
   <sheets>
     <sheet name="generador_datos" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="122">
   <si>
     <t>filtrar</t>
   </si>
@@ -168,58 +168,235 @@
     <t>Calidad</t>
   </si>
   <si>
-    <t>out_n_pedido_sap</t>
+    <t>strHoraCreado</t>
+  </si>
+  <si>
+    <t>strFechaCreado</t>
+  </si>
+  <si>
+    <t>strNumPedidoSap</t>
+  </si>
+  <si>
+    <t>strRefExterna</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>SI</t>
   </si>
   <si>
-    <t>out_ref_externa</t>
-  </si>
-  <si>
-    <t>LOTE1125</t>
-  </si>
-  <si>
-    <t>20200115</t>
-  </si>
-  <si>
-    <t>20210906</t>
-  </si>
-  <si>
-    <t>1125</t>
-  </si>
-  <si>
-    <t>R0000-00001125</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>20191116</t>
-  </si>
-  <si>
-    <t>3407077</t>
-  </si>
-  <si>
-    <t>1002;LOTE1125;20210906;DESC LOTE1125;LOTE1125;N;LOTE1125;;AR;;;;;;N;;;210;20181103;;N;</t>
-  </si>
-  <si>
-    <t>02000000001125;FNET;FNET;02;ZRET;20200115;;1800000122;20200115;08:00;16:00;20000;Remito electrónico Test;;;1002;27;C/U;LOTE1125;;;;;0000-00001125;1125;20200115;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIDO            20200115002C001CLIENTESAPNROOC032202001151002              27           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">202001150002073900PEDIDO                                                                          1002              27       139                         02        03      NUMEROWE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200115NROOC1  27     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              27     816 0  </t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>0001128513</t>
+    <t>27.01.2020</t>
+  </si>
+  <si>
+    <t>00:02</t>
+  </si>
+  <si>
+    <t>LOTE1179</t>
+  </si>
+  <si>
+    <t>20200127</t>
+  </si>
+  <si>
+    <t>20210918</t>
+  </si>
+  <si>
+    <t>1179</t>
+  </si>
+  <si>
+    <t>R0000-00001179</t>
+  </si>
+  <si>
+    <t>20191128</t>
+  </si>
+  <si>
+    <t>3407610</t>
+  </si>
+  <si>
+    <t>00:04</t>
+  </si>
+  <si>
+    <t>00:09</t>
+  </si>
+  <si>
+    <t>LOTE1181</t>
+  </si>
+  <si>
+    <t>1181</t>
+  </si>
+  <si>
+    <t>R0000-00001181</t>
+  </si>
+  <si>
+    <t>3407631</t>
+  </si>
+  <si>
+    <t>1002;LOTE1181;20210918;DESC LOTE1181;LOTE1181;N;LOTE1181;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001181;FNET;FNET;02;ZRET;20200127;;1800000122;20200127;08:00;16:00;20000;Remito electrónico Test;;;1002;25;C/U;LOTE1181;;;;;0000-00001181;1181;20200127;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200127002C001CLIENTESAPNROOC032202001271002              25           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202001270002073900PEDIDO                                                                          1002              25       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200127NROOC1  25     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              25     816 0  </t>
+  </si>
+  <si>
+    <t>00:19</t>
+  </si>
+  <si>
+    <t>LOTE1185</t>
+  </si>
+  <si>
+    <t>1185</t>
+  </si>
+  <si>
+    <t>R0000-00001185</t>
+  </si>
+  <si>
+    <t>3407673</t>
+  </si>
+  <si>
+    <t>1002;LOTE1185;20210918;DESC LOTE1185;LOTE1185;N;LOTE1185;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001185;FNET;FNET;02;ZRET;20200127;;1800000122;20200127;08:00;16:00;20000;Remito electrónico Test;;;1002;26;C/U;LOTE1185;;;;;0000-00001185;1185;20200127;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200127002C001CLIENTESAPNROOC032202001271002              26           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202001270002073900PEDIDO                                                                          1002              26       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200127NROOC1  26     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              26     816 0  </t>
+  </si>
+  <si>
+    <t>00:35</t>
+  </si>
+  <si>
+    <t>LOTE1189</t>
+  </si>
+  <si>
+    <t>1189</t>
+  </si>
+  <si>
+    <t>R0000-00001189</t>
+  </si>
+  <si>
+    <t>3407715</t>
+  </si>
+  <si>
+    <t>1002;LOTE1189;20210918;DESC LOTE1189;LOTE1189;N;LOTE1189;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001189;FNET;FNET;02;ZRET;20200127;;1800000122;20200127;08:00;16:00;20000;Remito electrónico Test;;;1002;27;C/U;LOTE1189;;;;;0000-00001189;1189;20200127;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200127002C001CLIENTESAPNROOC032202001271002              27           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202001270002073900PEDIDO                                                                          1002              27       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200127NROOC1  27     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              27     816 0  </t>
+  </si>
+  <si>
+    <t>00:46</t>
+  </si>
+  <si>
+    <t>LOTE1191</t>
+  </si>
+  <si>
+    <t>1191</t>
+  </si>
+  <si>
+    <t>R0000-00001191</t>
+  </si>
+  <si>
+    <t>3407736</t>
+  </si>
+  <si>
+    <t>1002;LOTE1191;20210918;DESC LOTE1191;LOTE1191;N;LOTE1191;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001191;FNET;FNET;02;ZRET;20200127;;1800000122;20200127;08:00;16:00;20000;Remito electrónico Test;;;1002;28;C/U;LOTE1191;;;;;0000-00001191;1191;20200127;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200127002C001CLIENTESAPNROOC032202001271002              28           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202001270002073900PEDIDO                                                                          1002              28       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200127NROOC1  28     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              28     816 0  </t>
+  </si>
+  <si>
+    <t>00:56</t>
+  </si>
+  <si>
+    <t>LOTE1193</t>
+  </si>
+  <si>
+    <t>1193</t>
+  </si>
+  <si>
+    <t>R0000-00001193</t>
+  </si>
+  <si>
+    <t>3407757</t>
+  </si>
+  <si>
+    <t>1002;LOTE1193;20210918;DESC LOTE1193;LOTE1193;N;LOTE1193;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001193;FNET;FNET;02;ZRET;20200127;;1800000122;20200127;08:00;16:00;20000;Remito electrónico Test;;;1002;29;C/U;LOTE1193;;;;;0000-00001193;1193;20200127;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200127002C001CLIENTESAPNROOC032202001271002              29           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202001270002073900PEDIDO                                                                          1002              29       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200127NROOC1  29     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              29     816 0  </t>
+  </si>
+  <si>
+    <t>01:07</t>
+  </si>
+  <si>
+    <t>LOTE1195</t>
+  </si>
+  <si>
+    <t>1195</t>
+  </si>
+  <si>
+    <t>R0000-00001195</t>
+  </si>
+  <si>
+    <t>3407778</t>
+  </si>
+  <si>
+    <t>1002;LOTE1195;20210918;DESC LOTE1195;LOTE1195;N;LOTE1195;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001195;FNET;FNET;02;ZRET;20200127;;1800000122;20200127;08:00;16:00;20000;Remito electrónico Test;;;1002;30;C/U;LOTE1195;;;;;0000-00001195;1195;20200127;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200127002C001CLIENTESAPNROOC032202001271002              30           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202001270002073900PEDIDO                                                                          1002              30       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200127NROOC1  30     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              30     816 0  </t>
   </si>
 </sst>
 </file>
@@ -227,10 +404,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -268,11 +451,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,57 +771,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2E8823-6EAB-486E-9169-DE992862E70B}">
-  <dimension ref="A1:AR2"/>
+  <dimension ref="A1:AT9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AN9" sqref="AN9"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="14.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="11" max="12" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="19" max="21" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="25.42578125" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="35" max="36" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="40" max="40" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="24.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="20" max="22" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -756,10 +944,10 @@
         <v>40</v>
       </c>
       <c r="AN1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>41</v>
@@ -770,8 +958,14 @@
       <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="AS1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -781,68 +975,631 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="L2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="M2">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="O2" t="s">
         <v>3</v>
       </c>
       <c r="W2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="X2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Y2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="Z2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="AD2">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="AG2">
         <v>2032500</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AI2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4">
+        <v>1128614</v>
+      </c>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>1002</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" t="s">
         <v>56</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="L3" t="s">
         <v>57</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="M3">
+        <v>24</v>
+      </c>
+      <c r="N3" t="s">
         <v>58</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="W3" t="s">
+        <v>50</v>
+      </c>
+      <c r="X3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y3" t="s">
         <v>59</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="Z3" t="s">
         <v>60</v>
       </c>
-      <c r="AN2">
-        <v>3407087</v>
-      </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AD3">
+        <v>24</v>
+      </c>
+      <c r="AG3">
+        <v>2032500</v>
+      </c>
+      <c r="AI3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="4"/>
+      <c r="AP3" s="4"/>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>1002</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4">
+        <v>25</v>
+      </c>
+      <c r="N4" t="s">
+        <v>65</v>
+      </c>
+      <c r="W4" t="s">
+        <v>50</v>
+      </c>
+      <c r="X4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD4">
+        <v>25</v>
+      </c>
+      <c r="AG4">
+        <v>2032500</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="4"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT4" s="3" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>1002</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5">
+        <v>26</v>
+      </c>
+      <c r="N5" t="s">
+        <v>75</v>
+      </c>
+      <c r="W5" t="s">
+        <v>50</v>
+      </c>
+      <c r="X5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD5">
+        <v>26</v>
+      </c>
+      <c r="AG5">
+        <v>2032500</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="4"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <v>1002</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6">
+        <v>27</v>
+      </c>
+      <c r="N6" t="s">
+        <v>85</v>
+      </c>
+      <c r="W6" t="s">
+        <v>50</v>
+      </c>
+      <c r="X6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD6">
+        <v>27</v>
+      </c>
+      <c r="AG6">
+        <v>2032500</v>
+      </c>
+      <c r="AI6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AL6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="4"/>
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="4"/>
+      <c r="AS6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT6" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>1002</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" t="s">
+        <v>94</v>
+      </c>
+      <c r="M7">
+        <v>28</v>
+      </c>
+      <c r="N7" t="s">
+        <v>95</v>
+      </c>
+      <c r="W7" t="s">
+        <v>50</v>
+      </c>
+      <c r="X7" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD7">
+        <v>28</v>
+      </c>
+      <c r="AG7">
+        <v>2032500</v>
+      </c>
+      <c r="AI7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AL7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AM7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AN7" s="4"/>
+      <c r="AO7" s="4"/>
+      <c r="AP7" s="4"/>
+      <c r="AQ7" s="4"/>
+      <c r="AR7" s="4"/>
+      <c r="AS7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT7" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8">
+        <v>1002</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8">
+        <v>29</v>
+      </c>
+      <c r="N8" t="s">
+        <v>105</v>
+      </c>
+      <c r="W8" t="s">
+        <v>50</v>
+      </c>
+      <c r="X8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD8">
+        <v>29</v>
+      </c>
+      <c r="AG8">
+        <v>2032500</v>
+      </c>
+      <c r="AI8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ8" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK8" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL8" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM8" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AN8" s="4"/>
+      <c r="AO8" s="4"/>
+      <c r="AP8" s="4"/>
+      <c r="AQ8" s="4"/>
+      <c r="AR8" s="4"/>
+      <c r="AS8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT8" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>1002</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" t="s">
+        <v>113</v>
+      </c>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" t="s">
+        <v>114</v>
+      </c>
+      <c r="M9">
+        <v>30</v>
+      </c>
+      <c r="N9" t="s">
+        <v>115</v>
+      </c>
+      <c r="W9" t="s">
+        <v>50</v>
+      </c>
+      <c r="X9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD9">
+        <v>30</v>
+      </c>
+      <c r="AG9">
+        <v>2032500</v>
+      </c>
+      <c r="AI9" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ9" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK9" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AL9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AM9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="AN9" s="4"/>
+      <c r="AO9" s="4"/>
+      <c r="AP9" s="4"/>
+      <c r="AQ9" s="4"/>
+      <c r="AR9" s="4"/>
+      <c r="AS9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT9" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPDATE: creacion scripts mm02 xd02 y mant de sen16
</commit_message>
<xml_diff>
--- a/Resources/db_farmanet_escenarios.xlsx
+++ b/Resources/db_farmanet_escenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alflopez-ext\Documents\Automation\Proyectos_Katalon\git\katalonProjects\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D302DABB-D6C0-48D2-811C-A34EA549F945}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C0B5A5-3C47-4B09-A527-2C939CAA004E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{DCE7E561-B195-4D45-B807-475C6552309D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
   <si>
     <t>filtrar</t>
   </si>
@@ -180,223 +180,115 @@
     <t>strRefExterna</t>
   </si>
   <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>28.01.2020</t>
+  </si>
+  <si>
+    <t>10:11</t>
+  </si>
+  <si>
+    <t>LOTE1197</t>
+  </si>
+  <si>
+    <t>20200128</t>
+  </si>
+  <si>
+    <t>20210919</t>
+  </si>
+  <si>
+    <t>1197</t>
+  </si>
+  <si>
+    <t>R0000-00001197</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>20191129</t>
+  </si>
+  <si>
+    <t>3407799</t>
+  </si>
+  <si>
+    <t>1002;LOTE1197;20210919;DESC LOTE1197;LOTE1197;N;LOTE1197;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001197;FNET;FNET;02;ZRET;20200128;;1800000122;20200128;08:00;16:00;20000;Remito electrónico Test;;;1002;10;C/U;LOTE1197;;;;;0000-00001197;1197;20200128;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200128002C001CLIENTESAPNROOC032202001281002              10           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202001280002073900PEDIDO                                                                          1002              10       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200128NROOC1  10     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              10     816 0  </t>
+  </si>
+  <si>
+    <t>10:22</t>
+  </si>
+  <si>
+    <t>LOTE1199</t>
+  </si>
+  <si>
+    <t>1199</t>
+  </si>
+  <si>
+    <t>R0000-00001199</t>
+  </si>
+  <si>
+    <t>3407820</t>
+  </si>
+  <si>
+    <t>1002;LOTE1199;20210919;DESC LOTE1199;LOTE1199;N;LOTE1199;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001199;FNET;FNET;02;ZRET;20200128;;1800000122;20200128;08:00;16:00;20000;Remito electrónico Test;;;1002;11;C/U;LOTE1199;;;;;0000-00001199;1199;20200128;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200128002C001CLIENTESAPNROOC032202001281002              11           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202001280002073900PEDIDO                                                                          1002              11       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200128NROOC1  11     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              11     816 0  </t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>SI</t>
-  </si>
-  <si>
-    <t>27.01.2020</t>
-  </si>
-  <si>
-    <t>00:02</t>
-  </si>
-  <si>
-    <t>LOTE1179</t>
-  </si>
-  <si>
-    <t>20200127</t>
-  </si>
-  <si>
-    <t>20210918</t>
-  </si>
-  <si>
-    <t>1179</t>
-  </si>
-  <si>
-    <t>R0000-00001179</t>
-  </si>
-  <si>
-    <t>20191128</t>
-  </si>
-  <si>
-    <t>3407610</t>
-  </si>
-  <si>
-    <t>00:04</t>
-  </si>
-  <si>
-    <t>00:09</t>
-  </si>
-  <si>
-    <t>LOTE1181</t>
-  </si>
-  <si>
-    <t>1181</t>
-  </si>
-  <si>
-    <t>R0000-00001181</t>
-  </si>
-  <si>
-    <t>3407631</t>
-  </si>
-  <si>
-    <t>1002;LOTE1181;20210918;DESC LOTE1181;LOTE1181;N;LOTE1181;;AR;;;;;;N;;;210;20181103;;N;</t>
-  </si>
-  <si>
-    <t>02000000001181;FNET;FNET;02;ZRET;20200127;;1800000122;20200127;08:00;16:00;20000;Remito electrónico Test;;;1002;25;C/U;LOTE1181;;;;;0000-00001181;1181;20200127;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIDO            20200127002C001CLIENTESAPNROOC032202001271002              25           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">202001270002073900PEDIDO                                                                          1002              25       139                         02        03      NUMEROWE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200127NROOC1  25     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              25     816 0  </t>
-  </si>
-  <si>
-    <t>00:19</t>
-  </si>
-  <si>
-    <t>LOTE1185</t>
-  </si>
-  <si>
-    <t>1185</t>
-  </si>
-  <si>
-    <t>R0000-00001185</t>
-  </si>
-  <si>
-    <t>3407673</t>
-  </si>
-  <si>
-    <t>1002;LOTE1185;20210918;DESC LOTE1185;LOTE1185;N;LOTE1185;;AR;;;;;;N;;;210;20181103;;N;</t>
-  </si>
-  <si>
-    <t>02000000001185;FNET;FNET;02;ZRET;20200127;;1800000122;20200127;08:00;16:00;20000;Remito electrónico Test;;;1002;26;C/U;LOTE1185;;;;;0000-00001185;1185;20200127;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIDO            20200127002C001CLIENTESAPNROOC032202001271002              26           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">202001270002073900PEDIDO                                                                          1002              26       139                         02        03      NUMEROWE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200127NROOC1  26     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              26     816 0  </t>
-  </si>
-  <si>
-    <t>00:35</t>
-  </si>
-  <si>
-    <t>LOTE1189</t>
-  </si>
-  <si>
-    <t>1189</t>
-  </si>
-  <si>
-    <t>R0000-00001189</t>
-  </si>
-  <si>
-    <t>3407715</t>
-  </si>
-  <si>
-    <t>1002;LOTE1189;20210918;DESC LOTE1189;LOTE1189;N;LOTE1189;;AR;;;;;;N;;;210;20181103;;N;</t>
-  </si>
-  <si>
-    <t>02000000001189;FNET;FNET;02;ZRET;20200127;;1800000122;20200127;08:00;16:00;20000;Remito electrónico Test;;;1002;27;C/U;LOTE1189;;;;;0000-00001189;1189;20200127;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIDO            20200127002C001CLIENTESAPNROOC032202001271002              27           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">202001270002073900PEDIDO                                                                          1002              27       139                         02        03      NUMEROWE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200127NROOC1  27     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              27     816 0  </t>
-  </si>
-  <si>
-    <t>00:46</t>
-  </si>
-  <si>
-    <t>LOTE1191</t>
-  </si>
-  <si>
-    <t>1191</t>
-  </si>
-  <si>
-    <t>R0000-00001191</t>
-  </si>
-  <si>
-    <t>3407736</t>
-  </si>
-  <si>
-    <t>1002;LOTE1191;20210918;DESC LOTE1191;LOTE1191;N;LOTE1191;;AR;;;;;;N;;;210;20181103;;N;</t>
-  </si>
-  <si>
-    <t>02000000001191;FNET;FNET;02;ZRET;20200127;;1800000122;20200127;08:00;16:00;20000;Remito electrónico Test;;;1002;28;C/U;LOTE1191;;;;;0000-00001191;1191;20200127;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIDO            20200127002C001CLIENTESAPNROOC032202001271002              28           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">202001270002073900PEDIDO                                                                          1002              28       139                         02        03      NUMEROWE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200127NROOC1  28     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              28     816 0  </t>
-  </si>
-  <si>
-    <t>00:56</t>
-  </si>
-  <si>
-    <t>LOTE1193</t>
-  </si>
-  <si>
-    <t>1193</t>
-  </si>
-  <si>
-    <t>R0000-00001193</t>
-  </si>
-  <si>
-    <t>3407757</t>
-  </si>
-  <si>
-    <t>1002;LOTE1193;20210918;DESC LOTE1193;LOTE1193;N;LOTE1193;;AR;;;;;;N;;;210;20181103;;N;</t>
-  </si>
-  <si>
-    <t>02000000001193;FNET;FNET;02;ZRET;20200127;;1800000122;20200127;08:00;16:00;20000;Remito electrónico Test;;;1002;29;C/U;LOTE1193;;;;;0000-00001193;1193;20200127;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIDO            20200127002C001CLIENTESAPNROOC032202001271002              29           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">202001270002073900PEDIDO                                                                          1002              29       139                         02        03      NUMEROWE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200127NROOC1  29     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              29     816 0  </t>
-  </si>
-  <si>
-    <t>01:07</t>
-  </si>
-  <si>
-    <t>LOTE1195</t>
-  </si>
-  <si>
-    <t>1195</t>
-  </si>
-  <si>
-    <t>R0000-00001195</t>
-  </si>
-  <si>
-    <t>3407778</t>
-  </si>
-  <si>
-    <t>1002;LOTE1195;20210918;DESC LOTE1195;LOTE1195;N;LOTE1195;;AR;;;;;;N;;;210;20181103;;N;</t>
-  </si>
-  <si>
-    <t>02000000001195;FNET;FNET;02;ZRET;20200127;;1800000122;20200127;08:00;16:00;20000;Remito electrónico Test;;;1002;30;C/U;LOTE1195;;;;;0000-00001195;1195;20200127;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIDO            20200127002C001CLIENTESAPNROOC032202001271002              30           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">202001270002073900PEDIDO                                                                          1002              30       139                         02        03      NUMEROWE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200127NROOC1  30     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              30     816 0  </t>
+    <t>16:20</t>
+  </si>
+  <si>
+    <t>LOTE1201</t>
+  </si>
+  <si>
+    <t>1201</t>
+  </si>
+  <si>
+    <t>R0000-00001201</t>
+  </si>
+  <si>
+    <t>3407841</t>
+  </si>
+  <si>
+    <t>1002;LOTE1201;20210919;DESC LOTE1201;LOTE1201;N;LOTE1201;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001201;FNET;FNET;02;ZRET;20200128;;1800000122;20200128;08:00;16:00;20000;Remito electrónico Test;;;1002;12;C/U;LOTE1201;;;;;0000-00001201;1201;20200128;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200128002C001CLIENTESAPNROOC032202001281002              12           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202001280002073900PEDIDO                                                                          1002              12       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200128NROOC1  12     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              12     816 0  </t>
   </si>
 </sst>
 </file>
@@ -771,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2E8823-6EAB-486E-9169-DE992862E70B}">
-  <dimension ref="A1:AT9"/>
+  <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AE10" sqref="AE10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,77 +868,77 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s">
         <v>54</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>55</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
         <v>56</v>
-      </c>
-      <c r="L2" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2">
-        <v>23</v>
-      </c>
-      <c r="N2" t="s">
-        <v>58</v>
       </c>
       <c r="O2" t="s">
         <v>3</v>
       </c>
       <c r="W2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="Y2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z2" t="s">
         <v>59</v>
       </c>
-      <c r="Z2" t="s">
-        <v>60</v>
-      </c>
       <c r="AD2">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="AG2">
         <v>2032500</v>
       </c>
       <c r="AI2" s="4" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="AK2" s="4" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="AL2" s="4" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="AM2" s="4" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="AN2" s="4"/>
       <c r="AO2" s="4">
-        <v>1128614</v>
+        <v>1128658</v>
       </c>
       <c r="AP2" s="4"/>
       <c r="AQ2" s="4"/>
       <c r="AR2" s="4"/>
       <c r="AS2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AT2" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
@@ -1060,72 +952,77 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" t="s">
         <v>54</v>
       </c>
-      <c r="J3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K3" t="s">
-        <v>56</v>
-      </c>
       <c r="L3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3">
+        <v>11</v>
+      </c>
+      <c r="N3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" t="s">
         <v>57</v>
       </c>
-      <c r="M3">
-        <v>24</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="X3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y3" t="s">
         <v>58</v>
       </c>
-      <c r="W3" t="s">
-        <v>50</v>
-      </c>
-      <c r="X3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>59</v>
-      </c>
       <c r="Z3" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="AD3">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="AG3">
         <v>2032500</v>
       </c>
       <c r="AI3" s="4" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="AK3" s="4" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="AL3" s="4" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="AM3" s="4" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="AN3" s="4"/>
-      <c r="AO3" s="4"/>
+      <c r="AO3" s="4">
+        <v>1128662</v>
+      </c>
       <c r="AP3" s="4"/>
       <c r="AQ3" s="4"/>
       <c r="AR3" s="4"/>
       <c r="AS3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AT3" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
@@ -1139,61 +1036,64 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="J4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L4" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="M4">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="N4" t="s">
-        <v>65</v>
+        <v>79</v>
+      </c>
+      <c r="O4" t="s">
+        <v>3</v>
       </c>
       <c r="W4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="X4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="Y4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z4" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="AD4">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="AG4">
         <v>2032500</v>
       </c>
       <c r="AI4" s="4" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="AJ4" s="4" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="AK4" s="4" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="AL4" s="4" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="AM4" s="4" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="AN4" s="4"/>
       <c r="AO4" s="4"/>
@@ -1201,10 +1101,10 @@
       <c r="AQ4" s="4"/>
       <c r="AR4" s="4"/>
       <c r="AS4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
@@ -1218,73 +1118,34 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" t="s">
-        <v>56</v>
-      </c>
-      <c r="L5" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="M5">
-        <v>26</v>
-      </c>
-      <c r="N5" t="s">
-        <v>75</v>
-      </c>
-      <c r="W5" t="s">
-        <v>50</v>
-      </c>
-      <c r="X5" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>76</v>
+        <v>13</v>
+      </c>
+      <c r="O5" t="s">
+        <v>3</v>
       </c>
       <c r="AD5">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="AG5">
         <v>2032500</v>
       </c>
-      <c r="AI5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ5" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="AK5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM5" s="4" t="s">
-        <v>81</v>
-      </c>
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4"/>
       <c r="AN5" s="4"/>
       <c r="AO5" s="4"/>
       <c r="AP5" s="4"/>
       <c r="AQ5" s="4"/>
       <c r="AR5" s="4"/>
-      <c r="AS5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT5" s="3" t="s">
-        <v>72</v>
-      </c>
+      <c r="AT5" s="3"/>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1297,73 +1158,34 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" t="s">
-        <v>83</v>
-      </c>
-      <c r="J6" t="s">
-        <v>55</v>
-      </c>
-      <c r="K6" t="s">
-        <v>56</v>
-      </c>
-      <c r="L6" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="M6">
-        <v>27</v>
-      </c>
-      <c r="N6" t="s">
-        <v>85</v>
-      </c>
-      <c r="W6" t="s">
-        <v>50</v>
-      </c>
-      <c r="X6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>86</v>
+        <v>14</v>
+      </c>
+      <c r="O6" t="s">
+        <v>3</v>
       </c>
       <c r="AD6">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="AG6">
         <v>2032500</v>
       </c>
-      <c r="AI6" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ6" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AK6" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="AL6" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="AM6" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
+      <c r="AK6" s="4"/>
+      <c r="AL6" s="4"/>
+      <c r="AM6" s="4"/>
       <c r="AN6" s="4"/>
       <c r="AO6" s="4"/>
       <c r="AP6" s="4"/>
       <c r="AQ6" s="4"/>
       <c r="AR6" s="4"/>
-      <c r="AS6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT6" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="AT6" s="3"/>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1376,231 +1198,34 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" t="s">
-        <v>93</v>
-      </c>
-      <c r="J7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="M7">
-        <v>28</v>
-      </c>
-      <c r="N7" t="s">
-        <v>95</v>
-      </c>
-      <c r="W7" t="s">
-        <v>50</v>
-      </c>
-      <c r="X7" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>96</v>
+        <v>15</v>
+      </c>
+      <c r="O7" t="s">
+        <v>3</v>
       </c>
       <c r="AD7">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="AG7">
         <v>2032500</v>
       </c>
-      <c r="AI7" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AJ7" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="AK7" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="AL7" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="AM7" s="4" t="s">
-        <v>101</v>
-      </c>
+      <c r="AI7" s="4"/>
+      <c r="AJ7" s="4"/>
+      <c r="AK7" s="4"/>
+      <c r="AL7" s="4"/>
+      <c r="AM7" s="4"/>
       <c r="AN7" s="4"/>
       <c r="AO7" s="4"/>
       <c r="AP7" s="4"/>
       <c r="AQ7" s="4"/>
       <c r="AR7" s="4"/>
-      <c r="AS7" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT7" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8">
-        <v>1002</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" t="s">
-        <v>103</v>
-      </c>
-      <c r="J8" t="s">
-        <v>55</v>
-      </c>
-      <c r="K8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L8" t="s">
-        <v>104</v>
-      </c>
-      <c r="M8">
-        <v>29</v>
-      </c>
-      <c r="N8" t="s">
-        <v>105</v>
-      </c>
-      <c r="W8" t="s">
-        <v>50</v>
-      </c>
-      <c r="X8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD8">
-        <v>29</v>
-      </c>
-      <c r="AG8">
-        <v>2032500</v>
-      </c>
-      <c r="AI8" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ8" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="AK8" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="AL8" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM8" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AN8" s="4"/>
-      <c r="AO8" s="4"/>
-      <c r="AP8" s="4"/>
-      <c r="AQ8" s="4"/>
-      <c r="AR8" s="4"/>
-      <c r="AS8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT8" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9">
-        <v>1002</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" t="s">
-        <v>113</v>
-      </c>
-      <c r="J9" t="s">
-        <v>55</v>
-      </c>
-      <c r="K9" t="s">
-        <v>56</v>
-      </c>
-      <c r="L9" t="s">
-        <v>114</v>
-      </c>
-      <c r="M9">
-        <v>30</v>
-      </c>
-      <c r="N9" t="s">
-        <v>115</v>
-      </c>
-      <c r="W9" t="s">
-        <v>50</v>
-      </c>
-      <c r="X9" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD9">
-        <v>30</v>
-      </c>
-      <c r="AG9">
-        <v>2032500</v>
-      </c>
-      <c r="AI9" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ9" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="AK9" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AL9" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="AM9" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="AN9" s="4"/>
-      <c r="AO9" s="4"/>
-      <c r="AP9" s="4"/>
-      <c r="AQ9" s="4"/>
-      <c r="AR9" s="4"/>
-      <c r="AS9" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT9" s="3" t="s">
-        <v>112</v>
-      </c>
+      <c r="AT7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UPDATE: guardados de n° de pedido, script para mm02, xd02, se16n lips
</commit_message>
<xml_diff>
--- a/Resources/db_farmanet_escenarios.xlsx
+++ b/Resources/db_farmanet_escenarios.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alflopez-ext\Documents\Automation\Proyectos_Katalon\git\katalonProjects\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C0B5A5-3C47-4B09-A527-2C939CAA004E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73BD343-D248-49EF-BB62-121AC812EEB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{DCE7E561-B195-4D45-B807-475C6552309D}"/>
   </bookViews>
   <sheets>
     <sheet name="generador_datos" sheetId="1" r:id="rId1"/>
+    <sheet name="mm02" sheetId="2" r:id="rId2"/>
+    <sheet name="xd02" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
   <si>
     <t>filtrar</t>
   </si>
@@ -156,9 +158,6 @@
     <t>out_ped_comitente_i101</t>
   </si>
   <si>
-    <t>out_n_entrega</t>
-  </si>
-  <si>
     <t>out_n_factura</t>
   </si>
   <si>
@@ -174,121 +173,156 @@
     <t>strFechaCreado</t>
   </si>
   <si>
-    <t>strNumPedidoSap</t>
-  </si>
-  <si>
     <t>strRefExterna</t>
   </si>
   <si>
     <t>SI</t>
   </si>
   <si>
-    <t>28.01.2020</t>
-  </si>
-  <si>
-    <t>10:11</t>
-  </si>
-  <si>
-    <t>LOTE1197</t>
-  </si>
-  <si>
-    <t>20200128</t>
-  </si>
-  <si>
-    <t>20210919</t>
-  </si>
-  <si>
-    <t>1197</t>
-  </si>
-  <si>
-    <t>R0000-00001197</t>
+    <t>strNumPedidoSap89</t>
+  </si>
+  <si>
+    <t>strNumPedidoSap101</t>
+  </si>
+  <si>
+    <t>strNumPedidoSap106</t>
+  </si>
+  <si>
+    <t>refExternaRemito</t>
+  </si>
+  <si>
+    <t>02</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>20191129</t>
-  </si>
-  <si>
-    <t>3407799</t>
-  </si>
-  <si>
-    <t>1002;LOTE1197;20210919;DESC LOTE1197;LOTE1197;N;LOTE1197;;AR;;;;;;N;;;210;20181103;;N;</t>
-  </si>
-  <si>
-    <t>02000000001197;FNET;FNET;02;ZRET;20200128;;1800000122;20200128;08:00;16:00;20000;Remito electrónico Test;;;1002;10;C/U;LOTE1197;;;;;0000-00001197;1197;20200128;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIDO            20200128002C001CLIENTESAPNROOC032202001281002              10           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">202001280002073900PEDIDO                                                                          1002              10       139                         02        03      NUMEROWE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200128NROOC1  10     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              10     816 0  </t>
-  </si>
-  <si>
-    <t>10:22</t>
-  </si>
-  <si>
-    <t>LOTE1199</t>
-  </si>
-  <si>
-    <t>1199</t>
-  </si>
-  <si>
-    <t>R0000-00001199</t>
-  </si>
-  <si>
-    <t>3407820</t>
-  </si>
-  <si>
-    <t>1002;LOTE1199;20210919;DESC LOTE1199;LOTE1199;N;LOTE1199;;AR;;;;;;N;;;210;20181103;;N;</t>
-  </si>
-  <si>
-    <t>02000000001199;FNET;FNET;02;ZRET;20200128;;1800000122;20200128;08:00;16:00;20000;Remito electrónico Test;;;1002;11;C/U;LOTE1199;;;;;0000-00001199;1199;20200128;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIDO            20200128002C001CLIENTESAPNROOC032202001281002              11           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">202001280002073900PEDIDO                                                                          1002              11       139                         02        03      NUMEROWE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200128NROOC1  11     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              11     816 0  </t>
+    <t>03:10</t>
+  </si>
+  <si>
+    <t>03:20</t>
+  </si>
+  <si>
+    <t>10.02.2020</t>
+  </si>
+  <si>
+    <t>LOTE1363</t>
+  </si>
+  <si>
+    <t>20200210</t>
+  </si>
+  <si>
+    <t>20211002</t>
+  </si>
+  <si>
+    <t>1363</t>
+  </si>
+  <si>
+    <t>R0000-00001363</t>
+  </si>
+  <si>
+    <t>20191212</t>
+  </si>
+  <si>
+    <t>3409542</t>
+  </si>
+  <si>
+    <t>1002;LOTE1363;20211002;DESC LOTE1363;LOTE1363;N;LOTE1363;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001363;FNET;FNET;02;ZRET;20200210;;1800000122;20200210;08:00;16:00;20000;Remito electrónico Test;;;1002;10;C/U;LOTE1363;;;;;0000-00001363;1363;20200210;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200210002C001CLIENTESAPNROOC032202002101002              10           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202002100002073900PEDIDO                                                                          1002              10       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200210NROOC1  10     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              10     816 0  </t>
+  </si>
+  <si>
+    <t>LOTE1365</t>
+  </si>
+  <si>
+    <t>1365</t>
+  </si>
+  <si>
+    <t>R0000-00001365</t>
+  </si>
+  <si>
+    <t>3409563</t>
+  </si>
+  <si>
+    <t>1002;LOTE1365;20211002;DESC LOTE1365;LOTE1365;N;LOTE1365;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001365;FNET;FNET;02;ZRET;20200210;;1800000122;20200210;08:00;16:00;20000;Remito electrónico Test;;;1002;11;C/U;LOTE1365;;;;;0000-00001365;1365;20200210;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200210002C001CLIENTESAPNROOC032202002101002              11           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202002100002073900PEDIDO                                                                          1002              10       139                         02        03      NUMEROWE 
+202002100002073900PEDIDO                                                                          1002              11       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200210NROOC1  10     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              10     816 0  
+VTD02    133198CLIENTESAPC00120200210NROOC1  11     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              11     816 0  </t>
+  </si>
+  <si>
+    <t>0001128920</t>
+  </si>
+  <si>
+    <t>0001128919</t>
+  </si>
+  <si>
+    <t>0001128918</t>
+  </si>
+  <si>
+    <t>0001128923</t>
+  </si>
+  <si>
+    <t>0001128922</t>
+  </si>
+  <si>
+    <t>0001128921</t>
+  </si>
+  <si>
+    <t>02000000001363</t>
+  </si>
+  <si>
+    <t>4000006414</t>
+  </si>
+  <si>
+    <t>02000000001365</t>
+  </si>
+  <si>
+    <t>4000006415</t>
+  </si>
+  <si>
+    <t>out_n_entrega_89</t>
+  </si>
+  <si>
+    <t>out_n_entrega_101</t>
+  </si>
+  <si>
+    <t>out_n_entrega_106</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>16:20</t>
-  </si>
-  <si>
-    <t>LOTE1201</t>
-  </si>
-  <si>
-    <t>1201</t>
-  </si>
-  <si>
-    <t>R0000-00001201</t>
-  </si>
-  <si>
-    <t>3407841</t>
-  </si>
-  <si>
-    <t>1002;LOTE1201;20210919;DESC LOTE1201;LOTE1201;N;LOTE1201;;AR;;;;;;N;;;210;20181103;;N;</t>
-  </si>
-  <si>
-    <t>02000000001201;FNET;FNET;02;ZRET;20200128;;1800000122;20200128;08:00;16:00;20000;Remito electrónico Test;;;1002;12;C/U;LOTE1201;;;;;0000-00001201;1201;20200128;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIDO            20200128002C001CLIENTESAPNROOC032202001281002              12           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">202001280002073900PEDIDO                                                                          1002              12       139                         02        03      NUMEROWE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200128NROOC1  12     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              12     816 0  </t>
+    <t>80871628</t>
+  </si>
+  <si>
+    <t>80871626</t>
+  </si>
+  <si>
+    <t>80871629</t>
+  </si>
+  <si>
+    <t>80871627</t>
   </si>
 </sst>
 </file>
@@ -343,12 +377,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,17 +703,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2E8823-6EAB-486E-9169-DE992862E70B}">
-  <dimension ref="A1:AT7"/>
+  <dimension ref="A1:AY3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AD8" sqref="AD8"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AY11" sqref="AY11:AY12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="18.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="18.5703125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="16.5703125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="22.140625" collapsed="true"/>
@@ -703,28 +743,31 @@
     <col min="32" max="32" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
     <col min="33" max="33" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
     <col min="34" max="34" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="10" width="20.7109375" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" style="10" width="20.28515625" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" style="10" width="23.140625" collapsed="true"/>
     <col min="38" max="38" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
     <col min="39" max="39" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
     <col min="40" max="40" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="42" max="43" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="50" max="51" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -820,13 +863,13 @@
       <c r="AH1" t="s">
         <v>35</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="8" t="s">
         <v>38</v>
       </c>
       <c r="AL1" s="1" t="s">
@@ -836,75 +879,93 @@
         <v>40</v>
       </c>
       <c r="AN1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AO1" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="AP1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AS1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>43</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>44</v>
       </c>
       <c r="B2">
         <v>1002</v>
       </c>
+      <c r="C2" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="K2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="M2">
         <v>10</v>
       </c>
       <c r="N2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="O2" t="s">
         <v>3</v>
       </c>
       <c r="W2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="X2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Y2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="Z2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AD2">
         <v>10</v>
@@ -912,83 +973,102 @@
       <c r="AG2">
         <v>2032500</v>
       </c>
-      <c r="AI2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AI2" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AN2" s="4"/>
-      <c r="AO2" s="4">
-        <v>1128658</v>
-      </c>
-      <c r="AP2" s="4"/>
-      <c r="AQ2" s="4"/>
-      <c r="AR2" s="4"/>
-      <c r="AS2" t="s">
-        <v>50</v>
-      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN2" s="3"/>
+      <c r="AO2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS2" s="3"/>
       <c r="AT2" s="3" t="s">
-        <v>51</v>
+        <v>85</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AW2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>1002</v>
       </c>
+      <c r="C3" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="L3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="M3">
         <v>11</v>
       </c>
       <c r="N3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O3" t="s">
         <v>3</v>
       </c>
       <c r="W3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="X3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="Y3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="Z3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AD3">
         <v>11</v>
@@ -996,239 +1076,77 @@
       <c r="AG3">
         <v>2032500</v>
       </c>
-      <c r="AI3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="AL3" s="4" t="s">
+      <c r="AI3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AM3" s="4" t="s">
+      <c r="AJ3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="AN3" s="4"/>
-      <c r="AO3" s="4">
-        <v>1128662</v>
-      </c>
-      <c r="AP3" s="4"/>
-      <c r="AQ3" s="4"/>
-      <c r="AR3" s="4"/>
-      <c r="AS3" t="s">
-        <v>50</v>
-      </c>
+      <c r="AK3" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN3" s="3"/>
+      <c r="AO3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AS3" s="3"/>
       <c r="AT3" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4">
-        <v>1002</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" t="s">
-        <v>78</v>
-      </c>
-      <c r="M4">
-        <v>12</v>
-      </c>
-      <c r="N4" t="s">
-        <v>79</v>
-      </c>
-      <c r="O4" t="s">
-        <v>3</v>
-      </c>
-      <c r="W4" t="s">
-        <v>57</v>
-      </c>
-      <c r="X4" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD4">
-        <v>12</v>
-      </c>
-      <c r="AG4">
-        <v>2032500</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AK4" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AM4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN4" s="4"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4"/>
-      <c r="AQ4" s="4"/>
-      <c r="AR4" s="4"/>
-      <c r="AS4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5">
-        <v>1002</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" t="s">
-        <v>49</v>
-      </c>
-      <c r="M5">
-        <v>13</v>
-      </c>
-      <c r="O5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD5">
-        <v>13</v>
-      </c>
-      <c r="AG5">
-        <v>2032500</v>
-      </c>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="4"/>
-      <c r="AK5" s="4"/>
-      <c r="AL5" s="4"/>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="4"/>
-      <c r="AO5" s="4"/>
-      <c r="AP5" s="4"/>
-      <c r="AQ5" s="4"/>
-      <c r="AR5" s="4"/>
-      <c r="AT5" s="3"/>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6">
-        <v>1002</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M6">
-        <v>14</v>
-      </c>
-      <c r="O6" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD6">
-        <v>14</v>
-      </c>
-      <c r="AG6">
-        <v>2032500</v>
-      </c>
-      <c r="AI6" s="4"/>
-      <c r="AJ6" s="4"/>
-      <c r="AK6" s="4"/>
-      <c r="AL6" s="4"/>
-      <c r="AM6" s="4"/>
-      <c r="AN6" s="4"/>
-      <c r="AO6" s="4"/>
-      <c r="AP6" s="4"/>
-      <c r="AQ6" s="4"/>
-      <c r="AR6" s="4"/>
-      <c r="AT6" s="3"/>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7">
-        <v>1002</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" t="s">
-        <v>49</v>
-      </c>
-      <c r="M7">
-        <v>15</v>
-      </c>
-      <c r="O7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD7">
-        <v>15</v>
-      </c>
-      <c r="AG7">
-        <v>2032500</v>
-      </c>
-      <c r="AI7" s="4"/>
-      <c r="AJ7" s="4"/>
-      <c r="AK7" s="4"/>
-      <c r="AL7" s="4"/>
-      <c r="AM7" s="4"/>
-      <c r="AN7" s="4"/>
-      <c r="AO7" s="4"/>
-      <c r="AP7" s="4"/>
-      <c r="AQ7" s="4"/>
-      <c r="AR7" s="4"/>
-      <c r="AT7" s="3"/>
+        <v>87</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AW3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF89BE5-456F-4275-8677-487AFC1C01B9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF51992A-29F9-430C-ADF2-09C7754697EB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
UPDATE: creacion se37 y we19 y mantenimiento general
</commit_message>
<xml_diff>
--- a/Resources/db_farmanet_escenarios.xlsx
+++ b/Resources/db_farmanet_escenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alflopez-ext\Documents\Automation\Proyectos_Katalon\git\katalonProjects\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73BD343-D248-49EF-BB62-121AC812EEB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FCC371-12C2-4308-90FE-7F636ED7ADA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{DCE7E561-B195-4D45-B807-475C6552309D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="175">
   <si>
     <t>filtrar</t>
   </si>
@@ -194,135 +194,382 @@
     <t>02</t>
   </si>
   <si>
+    <t>out_n_entrega_89</t>
+  </si>
+  <si>
+    <t>out_n_entrega_101</t>
+  </si>
+  <si>
+    <t>out_n_entrega_106</t>
+  </si>
+  <si>
+    <t>ingreso_123</t>
+  </si>
+  <si>
+    <t>param_material</t>
+  </si>
+  <si>
+    <t>param_cliente</t>
+  </si>
+  <si>
+    <t>egreso_125</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>03:10</t>
-  </si>
-  <si>
-    <t>03:20</t>
-  </si>
-  <si>
-    <t>10.02.2020</t>
-  </si>
-  <si>
-    <t>LOTE1363</t>
-  </si>
-  <si>
-    <t>20200210</t>
-  </si>
-  <si>
-    <t>20211002</t>
-  </si>
-  <si>
-    <t>1363</t>
-  </si>
-  <si>
-    <t>R0000-00001363</t>
-  </si>
-  <si>
-    <t>20191212</t>
-  </si>
-  <si>
-    <t>3409542</t>
-  </si>
-  <si>
-    <t>1002;LOTE1363;20211002;DESC LOTE1363;LOTE1363;N;LOTE1363;;AR;;;;;;N;;;210;20181103;;N;</t>
-  </si>
-  <si>
-    <t>02000000001363;FNET;FNET;02;ZRET;20200210;;1800000122;20200210;08:00;16:00;20000;Remito electrónico Test;;;1002;10;C/U;LOTE1363;;;;;0000-00001363;1363;20200210;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIDO            20200210002C001CLIENTESAPNROOC032202002101002              10           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">202002100002073900PEDIDO                                                                          1002              10       139                         02        03      NUMEROWE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200210NROOC1  10     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              10     816 0  </t>
-  </si>
-  <si>
-    <t>LOTE1365</t>
-  </si>
-  <si>
-    <t>1365</t>
-  </si>
-  <si>
-    <t>R0000-00001365</t>
-  </si>
-  <si>
-    <t>3409563</t>
-  </si>
-  <si>
-    <t>1002;LOTE1365;20211002;DESC LOTE1365;LOTE1365;N;LOTE1365;;AR;;;;;;N;;;210;20181103;;N;</t>
-  </si>
-  <si>
-    <t>02000000001365;FNET;FNET;02;ZRET;20200210;;1800000122;20200210;08:00;16:00;20000;Remito electrónico Test;;;1002;11;C/U;LOTE1365;;;;;0000-00001365;1365;20200210;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEDIDO            20200210002C001CLIENTESAPNROOC032202002101002              11           </t>
-  </si>
-  <si>
-    <t xml:space="preserve">202002100002073900PEDIDO                                                                          1002              10       139                         02        03      NUMEROWE 
-202002100002073900PEDIDO                                                                          1002              11       139                         02        03      NUMEROWE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200210NROOC1  10     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              10     816 0  
-VTD02    133198CLIENTESAPC00120200210NROOC1  11     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              11     816 0  </t>
-  </si>
-  <si>
-    <t>0001128920</t>
-  </si>
-  <si>
-    <t>0001128919</t>
-  </si>
-  <si>
-    <t>0001128918</t>
-  </si>
-  <si>
-    <t>0001128923</t>
-  </si>
-  <si>
-    <t>0001128922</t>
-  </si>
-  <si>
-    <t>0001128921</t>
-  </si>
-  <si>
-    <t>02000000001363</t>
-  </si>
-  <si>
-    <t>4000006414</t>
-  </si>
-  <si>
-    <t>02000000001365</t>
-  </si>
-  <si>
-    <t>4000006415</t>
-  </si>
-  <si>
-    <t>out_n_entrega_89</t>
-  </si>
-  <si>
-    <t>out_n_entrega_101</t>
-  </si>
-  <si>
-    <t>out_n_entrega_106</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>80871628</t>
-  </si>
-  <si>
-    <t>80871626</t>
-  </si>
-  <si>
-    <t>80871629</t>
-  </si>
-  <si>
-    <t>80871627</t>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>19.02.2020</t>
+  </si>
+  <si>
+    <t>11:04</t>
+  </si>
+  <si>
+    <t>LOTE1423</t>
+  </si>
+  <si>
+    <t>20200219</t>
+  </si>
+  <si>
+    <t>20211011</t>
+  </si>
+  <si>
+    <t>1423</t>
+  </si>
+  <si>
+    <t>0000R00001423</t>
+  </si>
+  <si>
+    <t>20191221</t>
+  </si>
+  <si>
+    <t>3410168</t>
+  </si>
+  <si>
+    <t>1002;LOTE1423;20211011;DESC LOTE1423;LOTE1423;N;LOTE1423;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001423;FNET;FNET;02;ZRET;20200219;;1800000122;20200219;08:00;16:00;20000;Remito electrónico Test;;;1002;10;C/U;LOTE1423;;;;;0000-00001423;1423;20200219;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200219002C001CLIENTESAPNROOC032202002191002              10           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202002190002073900PEDIDO                                                                          1002              10       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200219NROOC1  10     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              10     816 0  011   </t>
+  </si>
+  <si>
+    <t>11:14</t>
+  </si>
+  <si>
+    <t>LOTE1425</t>
+  </si>
+  <si>
+    <t>1425</t>
+  </si>
+  <si>
+    <t>0000R00001425</t>
+  </si>
+  <si>
+    <t>3410189</t>
+  </si>
+  <si>
+    <t>1002;LOTE1425;20211011;DESC LOTE1425;LOTE1425;N;LOTE1425;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001425;FNET;FNET;02;ZRET;20200219;;1800000122;20200219;08:00;16:00;20000;Remito electrónico Test;;;1002;11;C/U;LOTE1425;;;;;0000-00001425;1425;20200219;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200219002C001CLIENTESAPNROOC032202002191002              11           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202002190002073900PEDIDO                                                                          1002              10       139                         02        03      NUMEROWE 
+202002190002073900PEDIDO                                                                          1002              11       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200219NROOC1  10     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              10     816 0  011   
+VTD02    133198CLIENTESAPC00120200219NROOC1  11     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              11     816 0  011   </t>
+  </si>
+  <si>
+    <t>11:24</t>
+  </si>
+  <si>
+    <t>LOTE1427</t>
+  </si>
+  <si>
+    <t>1427</t>
+  </si>
+  <si>
+    <t>0000R00001427</t>
+  </si>
+  <si>
+    <t>3410210</t>
+  </si>
+  <si>
+    <t>1004;LOTE1427;20211011;DESC LOTE1427;LOTE1427;N;LOTE1427;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001427;FNET;FNET;02;ZRET;20200219;;1800000122;20200219;08:00;16:00;20000;Remito electrónico Test;;;1004;12;C/U;LOTE1427;;;;;0000-00001427;1427;20200219;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200219002C001CLIENTESAPNROOC032202002191004              12           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202002190002073900PEDIDO                                                                          1002              10       139                         02        03      NUMEROWE 
+202002190002073900PEDIDO                                                                          1002              11       139                         02        03      NUMEROWE 
+202002190002073900PEDIDO                                                                          1004              12       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200219NROOC1  10     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              10     816 0  011   
+VTD02    133198CLIENTESAPC00120200219NROOC1  11     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              11     816 0  011   
+VTD02    133198CLIENTESAPC00120200219NROOC1  12     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1004              12     816 0  011   </t>
+  </si>
+  <si>
+    <t>0001129310</t>
+  </si>
+  <si>
+    <t>0001129309</t>
+  </si>
+  <si>
+    <t>0001129311</t>
+  </si>
+  <si>
+    <t>0001129314</t>
+  </si>
+  <si>
+    <t>0001129313</t>
+  </si>
+  <si>
+    <t>0001129312</t>
+  </si>
+  <si>
+    <t>0001129315</t>
+  </si>
+  <si>
+    <t>0001129316</t>
+  </si>
+  <si>
+    <t>0001129317</t>
+  </si>
+  <si>
+    <t>02000000001423</t>
+  </si>
+  <si>
+    <t>4000006442</t>
+  </si>
+  <si>
+    <t>02000000001425</t>
+  </si>
+  <si>
+    <t>4000006443</t>
+  </si>
+  <si>
+    <t>02000000001427</t>
+  </si>
+  <si>
+    <t>4000006444</t>
+  </si>
+  <si>
+    <t>80871710</t>
+  </si>
+  <si>
+    <t>80871709</t>
+  </si>
+  <si>
+    <t>80871706</t>
+  </si>
+  <si>
+    <t>80871712</t>
+  </si>
+  <si>
+    <t>80871711</t>
+  </si>
+  <si>
+    <t>80871707</t>
+  </si>
+  <si>
+    <t>80871713</t>
+  </si>
+  <si>
+    <t>80871714</t>
+  </si>
+  <si>
+    <t>80871708</t>
+  </si>
+  <si>
+    <t>20.02.2020</t>
+  </si>
+  <si>
+    <t>10:15</t>
+  </si>
+  <si>
+    <t>LOTE1429</t>
+  </si>
+  <si>
+    <t>20200220</t>
+  </si>
+  <si>
+    <t>20211012</t>
+  </si>
+  <si>
+    <t>1429</t>
+  </si>
+  <si>
+    <t>0000R00001429</t>
+  </si>
+  <si>
+    <t>20191222</t>
+  </si>
+  <si>
+    <t>3410231</t>
+  </si>
+  <si>
+    <t>1002;LOTE1429;20211012;DESC LOTE1429;LOTE1429;N;LOTE1429;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001429;FNET;FNET;02;ZRET;20200220;;1800000122;20200220;08:00;16:00;20000;Remito electrónico Test;;;1002;10;C/U;LOTE1429;;;;;0000-00001429;1429;20200220;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200220002C001CLIENTESAPNROOC032202002201002              10           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202002200002073900PEDIDO                                                                          1002              10       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200220NROOC1  10     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              10     816 0  011   </t>
+  </si>
+  <si>
+    <t>10:25</t>
+  </si>
+  <si>
+    <t>LOTE1431</t>
+  </si>
+  <si>
+    <t>1431</t>
+  </si>
+  <si>
+    <t>0000R00001431</t>
+  </si>
+  <si>
+    <t>3410252</t>
+  </si>
+  <si>
+    <t>1002;LOTE1431;20211012;DESC LOTE1431;LOTE1431;N;LOTE1431;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001431;FNET;FNET;02;ZRET;20200220;;1800000122;20200220;08:00;16:00;20000;Remito electrónico Test;;;1002;11;C/U;LOTE1431;;;;;0000-00001431;1431;20200220;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200220002C001CLIENTESAPNROOC032202002201002              11           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202002200002073900PEDIDO                                                                          1002              10       139                         02        03      NUMEROWE 
+202002200002073900PEDIDO                                                                          1002              11       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200220NROOC1  10     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              10     816 0  011   
+VTD02    133198CLIENTESAPC00120200220NROOC1  11     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              11     816 0  011   </t>
+  </si>
+  <si>
+    <t>10:35</t>
+  </si>
+  <si>
+    <t>LOTE1433</t>
+  </si>
+  <si>
+    <t>1433</t>
+  </si>
+  <si>
+    <t>0000R00001433</t>
+  </si>
+  <si>
+    <t>3410273</t>
+  </si>
+  <si>
+    <t>1004;LOTE1433;20211012;DESC LOTE1433;LOTE1433;N;LOTE1433;;AR;;;;;;N;;;210;20181103;;N;</t>
+  </si>
+  <si>
+    <t>02000000001433;FNET;FNET;02;ZRET;20200220;;1800000122;20200220;08:00;16:00;20000;Remito electrónico Test;;;1004;12;C/U;LOTE1433;;;;;0000-00001433;1433;20200220;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEDIDO            20200220002C001CLIENTESAPNROOC032202002201004              12           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">202002200002073900PEDIDO                                                                          1002              10       139                         02        03      NUMEROWE 
+202002200002073900PEDIDO                                                                          1002              11       139                         02        03      NUMEROWE 
+202002200002073900PEDIDO                                                                          1004              12       139                         02        03      NUMEROWE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTD02    133198CLIENTESAPC00120200220NROOC1  10     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              10     816 0  011   
+VTD02    133198CLIENTESAPC00120200220NROOC1  11     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1002              11     816 0  011   
+VTD02    133198CLIENTESAPC00120200220NROOC1  12     /////ESTE PEDIDO HA SIDO CREADO POR UN PROCESO DE AUTOMATIZACION./////                    1004              12     816 0  011   </t>
+  </si>
+  <si>
+    <t>0001129355</t>
+  </si>
+  <si>
+    <t>0001129353</t>
+  </si>
+  <si>
+    <t>0001129354</t>
+  </si>
+  <si>
+    <t>0001129358</t>
+  </si>
+  <si>
+    <t>0001129356</t>
+  </si>
+  <si>
+    <t>0001129357</t>
+  </si>
+  <si>
+    <t>0001129361</t>
+  </si>
+  <si>
+    <t>0001129359</t>
+  </si>
+  <si>
+    <t>0001129360</t>
+  </si>
+  <si>
+    <t>02000000001429</t>
+  </si>
+  <si>
+    <t>4000006445</t>
+  </si>
+  <si>
+    <t>02000000001431</t>
+  </si>
+  <si>
+    <t>4000006446</t>
+  </si>
+  <si>
+    <t>02000000001433</t>
+  </si>
+  <si>
+    <t>4000006447</t>
+  </si>
+  <si>
+    <t>80871747</t>
+  </si>
+  <si>
+    <t>80871748</t>
+  </si>
+  <si>
+    <t>80871749</t>
+  </si>
+  <si>
+    <t>80871750</t>
+  </si>
+  <si>
+    <t>80871751</t>
+  </si>
+  <si>
+    <t>80871752</t>
   </si>
 </sst>
 </file>
@@ -377,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -389,6 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2E8823-6EAB-486E-9169-DE992862E70B}">
-  <dimension ref="A1:AY3"/>
+  <dimension ref="A1:BA4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AY11" sqref="AY11:AY12"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BB10" sqref="BB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,9 +1006,11 @@
     <col min="48" max="48" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
     <col min="49" max="49" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
     <col min="50" max="51" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -891,7 +1141,7 @@
         <v>50</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>41</v>
@@ -909,13 +1159,19 @@
         <v>51</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>90</v>
+        <v>55</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -935,37 +1191,37 @@
         <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="J2" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="K2" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="L2" t="s">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="M2">
         <v>10</v>
       </c>
       <c r="N2" t="s">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="O2" t="s">
         <v>3</v>
       </c>
       <c r="W2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="X2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="Y2" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="Z2" t="s">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="AD2">
         <v>10</v>
@@ -974,51 +1230,60 @@
         <v>2032500</v>
       </c>
       <c r="AI2" s="9" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="AJ2" s="9" t="s">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="AK2" s="9" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="AN2" s="3"/>
       <c r="AO2" s="4" t="s">
-        <v>78</v>
+        <v>154</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>79</v>
+        <v>155</v>
       </c>
       <c r="AQ2" s="5" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="AR2" t="s">
-        <v>92</v>
+        <v>169</v>
       </c>
       <c r="AS2" s="3"/>
       <c r="AT2" s="3" t="s">
-        <v>85</v>
+        <v>164</v>
       </c>
       <c r="AU2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>54</v>
+        <v>120</v>
+      </c>
+      <c r="AV2" s="11" t="s">
+        <v>121</v>
       </c>
       <c r="AW2" s="5" t="s">
-        <v>84</v>
+        <v>163</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>170</v>
       </c>
       <c r="AY2" t="s">
-        <v>93</v>
+        <v>113</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1038,37 +1303,37 @@
         <v>47</v>
       </c>
       <c r="I3" t="s">
-        <v>69</v>
+        <v>135</v>
       </c>
       <c r="J3" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="K3" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="L3" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="M3">
         <v>11</v>
       </c>
       <c r="N3" t="s">
-        <v>71</v>
+        <v>137</v>
       </c>
       <c r="O3" t="s">
         <v>3</v>
       </c>
       <c r="W3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="X3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="Y3" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="Z3" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="AD3">
         <v>11</v>
@@ -1077,48 +1342,169 @@
         <v>2032500</v>
       </c>
       <c r="AI3" s="9" t="s">
-        <v>73</v>
+        <v>139</v>
       </c>
       <c r="AJ3" s="9" t="s">
-        <v>74</v>
+        <v>140</v>
       </c>
       <c r="AK3" s="9" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="AM3" s="3" t="s">
-        <v>77</v>
+        <v>143</v>
       </c>
       <c r="AN3" s="3"/>
       <c r="AO3" s="4" t="s">
-        <v>81</v>
+        <v>157</v>
       </c>
       <c r="AP3" s="4" t="s">
-        <v>82</v>
+        <v>158</v>
       </c>
       <c r="AQ3" s="5" t="s">
-        <v>83</v>
+        <v>159</v>
       </c>
       <c r="AR3" t="s">
-        <v>94</v>
+        <v>171</v>
       </c>
       <c r="AS3" s="3"/>
       <c r="AT3" s="3" t="s">
-        <v>87</v>
+        <v>166</v>
       </c>
       <c r="AU3" t="s">
-        <v>56</v>
+        <v>120</v>
       </c>
       <c r="AV3" s="3" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="AW3" s="5" t="s">
-        <v>86</v>
+        <v>165</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>172</v>
       </c>
       <c r="AY3" t="s">
-        <v>95</v>
+        <v>116</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>1004</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" t="s">
+        <v>145</v>
+      </c>
+      <c r="J4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K4" t="s">
+        <v>124</v>
+      </c>
+      <c r="L4" t="s">
+        <v>146</v>
+      </c>
+      <c r="M4">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
+        <v>147</v>
+      </c>
+      <c r="O4" t="s">
+        <v>3</v>
+      </c>
+      <c r="W4" t="s">
+        <v>60</v>
+      </c>
+      <c r="X4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD4">
+        <v>12</v>
+      </c>
+      <c r="AG4">
+        <v>2032500</v>
+      </c>
+      <c r="AI4" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ4" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="AK4" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AP4" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="AQ4" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV4" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AW4" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>174</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1129,24 +1515,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF89BE5-456F-4275-8677-487AFC1C01B9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1572</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF51992A-29F9-430C-ADF2-09C7754697EB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5196903</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>